<commit_message>
Move supporting spreadsheets and info out of editing sheets
</commit_message>
<xml_diff>
--- a/scripts/AddictO_Table_Specifications.xlsx
+++ b/scripts/AddictO_Table_Specifications.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hastingj/Work/Onto/addiction-ontology/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E0DB05-D495-AE45-9467-C72DC5D0B2CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22452CE-1056-9641-839A-2CE6ECA7F5D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="-11860" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="-11080" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Classes worksheet key" sheetId="2" r:id="rId1"/>
-    <sheet name="Relations" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>ID</t>
   </si>
@@ -198,112 +197,19 @@
   </si>
   <si>
     <t>Enter an ontology entoty ID or a URI.</t>
-  </si>
-  <si>
-    <t>Parent relation</t>
-  </si>
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>Used in upper level</t>
-  </si>
-  <si>
-    <t>Subclass of</t>
-  </si>
-  <si>
-    <t>a subclass of b iff a and b are classes and b has all the properties of a and a does not have all the properties of b.</t>
-  </si>
-  <si>
-    <t>BFO</t>
-  </si>
-  <si>
-    <t>Studies</t>
-  </si>
-  <si>
-    <t>a studies b iff a is an agent and b is an entity where a  has a study investigator role in a research activity with the aim of gathering information about b.</t>
-  </si>
-  <si>
-    <t>Participant in (BFO)</t>
-  </si>
-  <si>
-    <t>Has behaviour</t>
-  </si>
-  <si>
-    <t>a has behaviour b iff a is a human being and b is a human behaviour and a is an agent that participates in b.</t>
-  </si>
-  <si>
-    <t>Participant in</t>
-  </si>
-  <si>
-    <t>BCIO</t>
-  </si>
-  <si>
-    <t>Environed in</t>
-  </si>
-  <si>
-    <t>a environed in b iff a is a material entity and b is an environmental system and a is located in the spatial region occupied by b and interacts with parts of b.</t>
-  </si>
-  <si>
-    <t>Has participant</t>
-  </si>
-  <si>
-    <t>A relation between a process and a continuant, in which the continuant is somehow involved in the process</t>
-  </si>
-  <si>
-    <t>RO</t>
-  </si>
-  <si>
-    <t>Has member</t>
-  </si>
-  <si>
-    <t>Has part</t>
-  </si>
-  <si>
-    <t>Produced by</t>
-  </si>
-  <si>
-    <t>Inverse of produces</t>
-  </si>
-  <si>
-    <t>Uses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a uses b iff a and b are participants in a behaviour in which a is an agent interacts with b in order to achieve a goal. </t>
-  </si>
-  <si>
-    <t>Interacts with</t>
-  </si>
-  <si>
-    <t>A relationship that holds between two entities in which the processes executed by the two entities are causally connected.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF222222"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -334,21 +240,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -633,235 +530,235 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="50.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="93" style="4" customWidth="1"/>
-    <col min="4" max="4" width="45.1640625" style="4" customWidth="1"/>
-    <col min="5" max="7" width="9.1640625" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" style="4"/>
+    <col min="1" max="1" width="27.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="93" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1640625" style="1" customWidth="1"/>
+    <col min="5" max="7" width="9.1640625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="1" t="s">
         <v>58</v>
       </c>
     </row>
@@ -869,203 +766,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.33203125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="36.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="37.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" style="1" customWidth="1"/>
-    <col min="13" max="15" width="9.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.1640625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="L9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>